<commit_message>
add poster to tasks
</commit_message>
<xml_diff>
--- a/progress_reports/tasks.xlsx
+++ b/progress_reports/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="53">
   <si>
     <t>Status</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Poster</t>
   </si>
 </sst>
 </file>
@@ -204,21 +207,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="7">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -234,18 +238,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -264,36 +261,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.39994506668294322"/>
@@ -301,153 +268,7 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -460,12 +281,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I35" totalsRowShown="0">
-  <autoFilter ref="A1:I35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I36" totalsRowShown="0">
+  <autoFilter ref="A1:I36"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="10" name="Done"/>
-    <tableColumn id="2" name="Status" dataDxfId="24">
+    <tableColumn id="2" name="Status" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Description"/>
@@ -766,7 +587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -775,7 +596,7 @@
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="12" bestFit="1" customWidth="1"/>
@@ -1301,107 +1122,110 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>24</v>
-      </c>
-      <c r="C22" t="str">
-        <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Ready</v>
+        <v>44</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
+        <v>Blocked</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="G22" t="s">
         <v>18</v>
+      </c>
+      <c r="H22">
+        <v>20</v>
+      </c>
+      <c r="I22">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C23" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Blocked</v>
+        <v>Ready</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
         <v>30</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23">
-        <v>24</v>
-      </c>
-      <c r="I23">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C24" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Ready</v>
+        <v>Blocked</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F24" t="s">
         <v>30</v>
       </c>
       <c r="G24" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H24">
+        <v>24</v>
+      </c>
+      <c r="I24">
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C25" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Blocked</v>
+        <v>Ready</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
         <v>30</v>
       </c>
       <c r="G25" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
         <v>Blocked</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
@@ -1413,43 +1237,46 @@
         <v>19</v>
       </c>
       <c r="H26">
-        <v>28</v>
-      </c>
-      <c r="I26">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C27" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Ready</v>
+        <v>Blocked</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F27" t="s">
         <v>30</v>
       </c>
       <c r="G27" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H27">
+        <v>28</v>
+      </c>
+      <c r="I27">
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Blocked</v>
+        <v>Ready</v>
       </c>
       <c r="D28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1460,20 +1287,17 @@
       <c r="G28" t="s">
         <v>18</v>
       </c>
-      <c r="H28">
-        <v>26</v>
-      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
         <v>Blocked</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1482,28 +1306,25 @@
         <v>30</v>
       </c>
       <c r="G29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H29">
-        <v>31</v>
-      </c>
-      <c r="I29">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C30" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
         <v>Blocked</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
         <v>30</v>
@@ -1512,40 +1333,46 @@
         <v>19</v>
       </c>
       <c r="H30">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="I30">
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C31" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Ready</v>
+        <v>Blocked</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G31" t="s">
         <v>19</v>
       </c>
+      <c r="H31">
+        <v>33</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Blocked</v>
+        <v>Ready</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1554,70 +1381,67 @@
         <v>40</v>
       </c>
       <c r="G32" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C33" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
         <v>Blocked</v>
       </c>
       <c r="D33" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F33" t="s">
         <v>40</v>
       </c>
       <c r="G33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H33">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C34" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
         <v>Blocked</v>
       </c>
       <c r="D34" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F34" t="s">
         <v>40</v>
       </c>
       <c r="G34" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H34">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
         <v>Blocked</v>
       </c>
       <c r="D35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1632,66 +1456,90 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="1">
-        <f>COUNTA(B2:B21)/ROWS(B2:B21)</f>
-        <v>0.1</v>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>43</v>
+      </c>
+      <c r="C36" t="str">
+        <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
+        <v>Blocked</v>
+      </c>
+      <c r="D36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36">
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B38" s="1">
-        <f>COUNTA(B22:B30)/ROWS(B22:B30)</f>
-        <v>0</v>
+        <f>COUNTA(B2:B22)/ROWS(B2:B22)</f>
+        <v>9.5238095238095233E-2</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B39" s="1">
-        <f>COUNTA(B31:B35)/ROWS(B31:B35)</f>
+        <f>COUNTA(B23:B31)/ROWS(B23:B31)</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="1">
+        <f>COUNTA(B32:B36)/ROWS(B32:B36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B41" s="1">
         <f>COUNTA(Table3[Done])/ROWS(Table3[Done])</f>
-        <v>5.8823529411764705E-2</v>
+        <v>5.7142857142857141E-2</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Tertiary"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Secondary"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"Primary"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
-      <formula>"Tertiary"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Ready"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
-      <formula>"Ready"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37:B40">
+  <conditionalFormatting sqref="B38:B41">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
remove duplicate task - design routing algorithm
</commit_message>
<xml_diff>
--- a/progress_reports/tasks.xlsx
+++ b/progress_reports/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="52">
   <si>
     <t>Status</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>Design encryption mechanism</t>
-  </si>
-  <si>
-    <t>Design routing algorithm</t>
   </si>
   <si>
     <t>Create a smartphone UI</t>
@@ -281,8 +278,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I36" totalsRowShown="0">
-  <autoFilter ref="A1:I36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I35" totalsRowShown="0">
+  <autoFilter ref="A1:I35"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="10" name="Done"/>
@@ -587,16 +584,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="46.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="12" bestFit="1" customWidth="1"/>
@@ -604,10 +603,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -640,7 +639,7 @@
         <v>Ready</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -661,7 +660,7 @@
         <v>Blocked</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -685,7 +684,7 @@
         <v>Blocked</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -801,7 +800,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
@@ -825,7 +824,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
@@ -1074,35 +1073,38 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Ready</v>
+        <v>Blocked</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
       </c>
       <c r="G20" t="s">
         <v>18</v>
+      </c>
+      <c r="H20">
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="C21" t="str">
+        <v>44</v>
+      </c>
+      <c r="C21" s="2" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
         <v>Blocked</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -1114,111 +1116,108 @@
         <v>18</v>
       </c>
       <c r="H21">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I21">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>44</v>
-      </c>
-      <c r="C22" s="2" t="str">
-        <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Blocked</v>
+        <v>24</v>
+      </c>
+      <c r="C22" t="str">
+        <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
+        <v>Ready</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="G22" t="s">
         <v>18</v>
-      </c>
-      <c r="H22">
-        <v>20</v>
-      </c>
-      <c r="I22">
-        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="C23" t="str">
+        <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
+        <v>Blocked</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23">
         <v>24</v>
       </c>
-      <c r="C23" t="str">
-        <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Ready</v>
-      </c>
-      <c r="D23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" t="s">
-        <v>18</v>
+      <c r="I23">
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C24" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Blocked</v>
+        <v>Ready</v>
       </c>
       <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
         <v>29</v>
       </c>
-      <c r="E24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" t="s">
-        <v>30</v>
-      </c>
       <c r="G24" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24">
-        <v>24</v>
-      </c>
-      <c r="I24">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C25" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Ready</v>
+        <v>Blocked</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G25" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H25">
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
@@ -1231,49 +1230,46 @@
         <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G26" t="s">
         <v>19</v>
       </c>
       <c r="H26">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="I26">
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C27" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Blocked</v>
+        <v>Ready</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G27" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27">
-        <v>28</v>
-      </c>
-      <c r="I27">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C28" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Ready</v>
+        <v>Blocked</v>
       </c>
       <c r="D28" t="s">
         <v>36</v>
@@ -1282,15 +1278,18 @@
         <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G28" t="s">
         <v>18</v>
+      </c>
+      <c r="H28">
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C29" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
@@ -1303,73 +1302,70 @@
         <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G29" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H29">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="I29">
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C30" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
         <v>Blocked</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G30" t="s">
         <v>19</v>
       </c>
       <c r="H30">
-        <v>31</v>
-      </c>
-      <c r="I30">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C31" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Blocked</v>
+        <v>Ready</v>
       </c>
       <c r="D31" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E31" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G31" t="s">
         <v>19</v>
       </c>
-      <c r="H31">
-        <v>33</v>
-      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C32" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Ready</v>
+        <v>Blocked</v>
       </c>
       <c r="D32" t="s">
         <v>41</v>
@@ -1378,63 +1374,66 @@
         <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G32" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="H32">
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
+        <v>35</v>
+      </c>
+      <c r="C33" t="str">
+        <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
+        <v>Blocked</v>
+      </c>
+      <c r="D33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33">
         <v>37</v>
-      </c>
-      <c r="C33" t="str">
-        <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Blocked</v>
-      </c>
-      <c r="D33" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" t="s">
-        <v>40</v>
-      </c>
-      <c r="G33" t="s">
-        <v>18</v>
-      </c>
-      <c r="H33">
-        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C34" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
         <v>Blocked</v>
       </c>
       <c r="D34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
         <v>39</v>
       </c>
-      <c r="E34" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" t="s">
-        <v>40</v>
-      </c>
       <c r="G34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H34">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C35" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
@@ -1447,7 +1446,7 @@
         <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G35" t="s">
         <v>18</v>
@@ -1456,64 +1455,40 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>43</v>
-      </c>
-      <c r="C36" t="str">
-        <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Blocked</v>
-      </c>
-      <c r="D36" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" t="s">
-        <v>40</v>
-      </c>
-      <c r="G36" t="s">
-        <v>18</v>
-      </c>
-      <c r="H36">
-        <v>23</v>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1">
+        <f>COUNTA(B2:B21)/ROWS(B2:B21)</f>
+        <v>0.1</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B38" s="1">
-        <f>COUNTA(B2:B22)/ROWS(B2:B22)</f>
-        <v>9.5238095238095233E-2</v>
+        <f>COUNTA(B22:B30)/ROWS(B22:B30)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1">
-        <f>COUNTA(B23:B31)/ROWS(B23:B31)</f>
+        <f>COUNTA(B31:B35)/ROWS(B31:B35)</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B40" s="1">
-        <f>COUNTA(B32:B36)/ROWS(B32:B36)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="1">
         <f>COUNTA(Table3[Done])/ROWS(Table3[Done])</f>
-        <v>5.7142857142857141E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1539,7 +1514,7 @@
       <formula>"Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38:B41">
+  <conditionalFormatting sqref="B37:B40">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
add to play store
</commit_message>
<xml_diff>
--- a/progress_reports/tasks.xlsx
+++ b/progress_reports/tasks.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ndw.home.cs.st-andrews.ac.uk\ndw\hg\sh-proj\progress_reports\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="51">
   <si>
     <t>Status</t>
   </si>
@@ -345,7 +340,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -380,7 +375,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -591,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,9 +1174,12 @@
       <c r="A22">
         <v>23</v>
       </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
       <c r="C22" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Ready</v>
+        <v>Done</v>
       </c>
       <c r="D22" t="s">
         <v>26</v>
@@ -1446,9 +1444,12 @@
       <c r="A33">
         <v>42</v>
       </c>
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
       <c r="C33" t="str">
         <f>IF(ISBLANK(Table3[[#This Row],[Done]]),IF(AND(IF(ISBLANK(Table3[[#This Row],[Depends0]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends0]],Table3[Number],0))))),IF(ISBLANK(Table3[[#This Row],[Depends1]]),TRUE,NOT(ISBLANK(INDEX(Table3[Done],MATCH(Table3[[#This Row],[Depends1]],Table3[Number],0)))))),"Ready","Blocked"),"Done")</f>
-        <v>Blocked</v>
+        <v>Done</v>
       </c>
       <c r="D33" t="s">
         <v>41</v>
@@ -1508,7 +1509,7 @@
       </c>
       <c r="B37" s="1">
         <f>COUNTA(B21:B29)/ROWS(B21:B29)</f>
-        <v>0.33333333333333331</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1517,7 +1518,7 @@
       </c>
       <c r="B38" s="1">
         <f>COUNTA(B30:B34)/ROWS(B30:B34)</f>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1526,7 +1527,7 @@
       </c>
       <c r="B39" s="1">
         <f>COUNTA(Table3[Done])/ROWS(Table3[Done])</f>
-        <v>0.66666666666666663</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
   </sheetData>

</xml_diff>